<commit_message>
More data from participants
</commit_message>
<xml_diff>
--- a/Last Experiment_ Post-Experiment Questionnaire (Responses).xlsx
+++ b/Last Experiment_ Post-Experiment Questionnaire (Responses).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="87">
   <si>
     <t>Timestamp</t>
   </si>
@@ -42,7 +42,8 @@
     <t>Define your level of experience with robotics:</t>
   </si>
   <si>
-    <t>(If applicable) What year are you in college?</t>
+    <t>(If applicable) What year are you in college?
+If you are not an undergraduate student, please use the Other field to indicate your status (e.g., Ph.D. Student, Masters Student, etc)</t>
   </si>
   <si>
     <t xml:space="preserve">(If applicable) When studying computer programming, what types of learning materials do you use the most?  </t>
@@ -91,6 +92,9 @@
 Keep in mind that by writing your name below, you allow us to save and share your name with your professor. Your name will not be used for research purposes, and will be deleted from our data once your professor is notified.</t>
   </si>
   <si>
+    <t>Do you have any positive or negative comments about the block-based language you used in this experiment? Feel free to share as many details are you want.</t>
+  </si>
+  <si>
     <t>p0410947</t>
   </si>
   <si>
@@ -100,7 +104,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>This participant used the first version of our experiment guidelines. I made minor changes in the first two paragraphs of the guidelines for the following participants. That may be the reason why he got confused.</t>
+    <t>This participant used the first version of our experiment guidelines. I made minor changes in the first two paragraphs of the guidelines for the following participants. That may be the reason why he got confused with the cans.</t>
   </si>
   <si>
     <t>1 - 3 years of programming experience</t>
@@ -133,6 +137,9 @@
     <t>i want to know the solution haha</t>
   </si>
   <si>
+    <t>This participant did not have this question available when they answer the survey.</t>
+  </si>
+  <si>
     <t>p04101103</t>
   </si>
   <si>
@@ -178,7 +185,7 @@
     <t>p04101549</t>
   </si>
   <si>
-    <t xml:space="preserve">The ABB Wizard Programming Tool stopped working, and the system was frozen. We had to restart the robot controller. It took about 3 minutes to restart the controller. I gave 3 minutes of extra time in the one hour limit. </t>
+    <t xml:space="preserve">The ABB Wizard Programming Tool stopped working, and the system was frozen. We had to restart the robot controller. It took about 3 minutes to restart the controller and get things back to normal. I gave 3 minutes of extra time in the one hour limit. </t>
   </si>
   <si>
     <t>1 - 3 years of experience</t>
@@ -203,6 +210,72 @@
   </si>
   <si>
     <t>Ishaan Chadha, Class:CMSC425</t>
+  </si>
+  <si>
+    <t>p04111055</t>
+  </si>
+  <si>
+    <t>4 - 5 years of programming experience</t>
+  </si>
+  <si>
+    <t>Moderate experience</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy), Online Communities (e.g., Reddit, Stack Overflow), Technical Documentation</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not always accessible, The information and resources are not organized into logical and understandable components</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not always accessible</t>
+  </si>
+  <si>
+    <t>it felt like there was no purpose to typing in a description of my question</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>it felt like the materials provided weren't relevant to the mechanics of the tablet</t>
+  </si>
+  <si>
+    <t>I think it was a good learning experience since i have never used the block format before</t>
+  </si>
+  <si>
+    <t>Matthew Xu CMSC 425</t>
+  </si>
+  <si>
+    <t>p04111301</t>
+  </si>
+  <si>
+    <t>The information and resources are not concise and clear, The information and resources are not organized into logical and understandable components</t>
+  </si>
+  <si>
+    <t>The block code was easy to use.</t>
+  </si>
+  <si>
+    <t>Michael Huynh</t>
+  </si>
+  <si>
+    <t>The block based code was easy to use and understand.</t>
+  </si>
+  <si>
+    <t>p04111434</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not in a form that is readily useable, The information and resources are not concise and clear</t>
+  </si>
+  <si>
+    <t>I only used the chat function, which was very useful in explaining and giving examples of what the robot is capable of and what to do with my ideas on how to implement the functions for the requirements.</t>
+  </si>
+  <si>
+    <t>I enjoy the simplicity that comes with block based coding, a simple swipe is enough to define a function and its uses, however, since I am not used to it I am not to versed in how to specify certain inputs with actions.</t>
+  </si>
+  <si>
+    <t>Sanie Fragata CMSC 425</t>
   </si>
 </sst>
 </file>
@@ -245,11 +318,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -478,7 +554,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="31" width="18.88"/>
+    <col customWidth="1" min="1" max="32" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -557,268 +633,496 @@
       <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>45392.457167430555</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="G2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="O2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="R2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>38</v>
+      <c r="U2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>45392.5118530787</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>45392.646322256944</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="M4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y4" s="3" t="s">
+      <c r="P4" s="4" t="s">
         <v>52</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>45392.71231827546</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="S5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>45393.51467798611</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="D6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="3" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>45393.603960092594</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="R5" s="3" t="s">
+      <c r="L7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>62</v>
+      <c r="P7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z7" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>45393.653702118056</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Last Experiment_ Post-Experiment Questionnaire (Responses).xlsx
</commit_message>
<xml_diff>
--- a/Last Experiment_ Post-Experiment Questionnaire (Responses).xlsx
+++ b/Last Experiment_ Post-Experiment Questionnaire (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conso\OneDrive\Documents\GitHub\robot-barriers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FF0A8A-6FCF-4082-9B24-36D5A51D6037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F25374-A8DD-4A2A-B7BF-CE84C82137AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="163">
   <si>
     <t>Timestamp</t>
   </si>
@@ -104,7 +104,7 @@
     <t>Do you have any positive or negative comments about the block-based language you used in this experiment? Feel free to share as many details are you want.</t>
   </si>
   <si>
-    <t>p0410947</t>
+    <t>p04100947</t>
   </si>
   <si>
     <t>Yes</t>
@@ -423,6 +423,102 @@
   </si>
   <si>
     <t xml:space="preserve">For someone with no experience I somewhat figured it out. </t>
+  </si>
+  <si>
+    <t>p04161322</t>
+  </si>
+  <si>
+    <t>Lecture Materials (e.g., In-Class Slides, Lecture Notes)</t>
+  </si>
+  <si>
+    <t>p04161834</t>
+  </si>
+  <si>
+    <t>Participant left early, spending 50 minutes in the experiment. He partially completed the task.</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not in a form that is readily useable, The information and resources are not concise and clear, The information and resources are not organized into logical and understandable components</t>
+  </si>
+  <si>
+    <t>I think my experience was good, I may have liked to have a partner or a 2nd thought on things.</t>
+  </si>
+  <si>
+    <t>I had a positive experience with the time I had, I had to leave early but putting together the block based language to see the robot arm moving the coffee cans was pretty cool.</t>
+  </si>
+  <si>
+    <t>p04171512</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy), Online Communities (e.g., Reddit, Stack Overflow), Chatbots (e.g., ChatGPT)</t>
+  </si>
+  <si>
+    <t>Needs more video representation</t>
+  </si>
+  <si>
+    <t>The chat bot was very responsive</t>
+  </si>
+  <si>
+    <t>Yes defintely couldve been clearer what the task is</t>
+  </si>
+  <si>
+    <t>The block language is pretty intuitive</t>
+  </si>
+  <si>
+    <t>p04171840</t>
+  </si>
+  <si>
+    <t>The proctor put the wrong ID for this participant (p04171950 is p04171840). The program would not let him apply any new work and froze for a bit. His code is based off his logic, not testing since the robot would not update with new code in the last 15 minutes.</t>
+  </si>
+  <si>
+    <t>Videos (e.g., YouTube, Udemy)</t>
+  </si>
+  <si>
+    <t>Watch</t>
+  </si>
+  <si>
+    <t>Videos were very helpful and programming the robot was easy.</t>
+  </si>
+  <si>
+    <t>The language is fine, just the robot did not apply the new code I gave him</t>
+  </si>
+  <si>
+    <t>p04181446</t>
+  </si>
+  <si>
+    <t>PhD student</t>
+  </si>
+  <si>
+    <t>The materials do not provide the sufficient or required information, The information and resources are not always accessible, The information and resources are not in a form that is readily useable, The information and resources are not concise and clear, The information and resources are not organized into logical and understandable components, The information and resources provided are not up to date</t>
+  </si>
+  <si>
+    <t>I did not study robot pogramming</t>
+  </si>
+  <si>
+    <t>The information and resources are not organized into logical and understandable components</t>
+  </si>
+  <si>
+    <t>I did not use them</t>
+  </si>
+  <si>
+    <t>The experiment was very well setup. I like that it required repetition while also changing some values that were repeated (i.e. location that the robot would put the cans in).
+Additionally, I liked that the experiment was challenging but also accessible. Especially for someone with some coding experience, but no robot coding experience.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I feel that the block based language is very easy to understand, especially for people who have a basic understanding of coding. 
+The block based language makes creating functions much easier, as repetitive tasks can be copied and dragged over. However, a user interacting with the block based language may struggle to understand how to duplicate blocks without guidance. 
+I think that the block based programming language would benefit a lot from a smoother display/machine that it is running on. Some issues I ran into would be maybe expecting to be able to pinch to zoom, or attempt to highlight a block and drag which I could not do. However this is a hardware issue, and not at all an issue with the block based language. </t>
+  </si>
+  <si>
+    <t>p04181705</t>
+  </si>
+  <si>
+    <t>More than 5 years of programming experience</t>
+  </si>
+  <si>
+    <t>The information and resources are not in a form that is readily useable, The information and resources are not concise and clear, The information and resources provided are not up to date</t>
+  </si>
+  <si>
+    <t>Even with my last experience with Scratch happened 7 years ago It was super easy to use the tool provided.</t>
   </si>
 </sst>
 </file>
@@ -695,11 +791,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2:Y17"/>
+      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2:Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1867,6 +1963,415 @@
         <v>131</v>
       </c>
     </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2">
+        <v>45398.458225312497</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2">
+        <v>45398.637042881943</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>45399.515523819442</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2">
+        <v>45399.66549944444</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2">
+        <v>45400.500941493054</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>45400.57352726852</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>